<commit_message>
input and button styled
</commit_message>
<xml_diff>
--- a/history.xlsx
+++ b/history.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -822,6 +822,75 @@
       <c r="E14" t="inlineStr">
         <is>
           <t>07/14/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Sarunas Stoncelis</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ref78999</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>8794</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>7685.3</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>07/26/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Jonathan Fire</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>paiment345</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0985</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>658</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>07/26/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>jjoo</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>07/26/2022</t>
         </is>
       </c>
     </row>

</xml_diff>